<commit_message>
test cases change: input added but no output
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zee/development/CS151_labs/Lab2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxrice/PycharmProjects/cs151-lab2-max-and-jenna/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C084CA8B-2F93-D948-9FA4-65E66A2852B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A353751-557C-BD4D-B085-D899F6D8DEBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="67920" windowHeight="28300" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19940" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -164,14 +164,14 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -197,9 +197,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -237,7 +237,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -343,7 +343,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -485,7 +485,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -496,7 +496,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:I10"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -509,44 +509,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <f>60*60*24*365</f>
         <v>31536000</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -564,98 +564,148 @@
       <c r="I4" s="5"/>
     </row>
     <row r="5" spans="1:9" ht="76" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="B6" s="1">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1">
+        <v>126</v>
+      </c>
+      <c r="E6" s="1">
+        <v>333100360</v>
+      </c>
+      <c r="F6" s="1">
+        <v>5</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
+      <c r="B7" s="1">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1">
+        <v>126</v>
+      </c>
+      <c r="E7" s="1">
+        <v>333100360</v>
+      </c>
+      <c r="F7" s="1">
+        <v>5</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
+      <c r="B8" s="1">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1">
+        <v>126</v>
+      </c>
+      <c r="E8" s="1">
+        <v>333100360</v>
+      </c>
+      <c r="F8" s="1">
+        <v>5</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+      <c r="B9" s="1">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1">
+        <v>126</v>
+      </c>
+      <c r="E9" s="1">
+        <v>333100360</v>
+      </c>
+      <c r="F9" s="1">
+        <v>5</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="B10" s="1">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1">
+        <v>12</v>
+      </c>
+      <c r="D10" s="1">
+        <v>200</v>
+      </c>
+      <c r="E10" s="1">
+        <v>333100360</v>
+      </c>
+      <c r="F10" s="1">
+        <v>5</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
filled in some test cases
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxrice/PycharmProjects/cs151-lab2-max-and-jenna/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A353751-557C-BD4D-B085-D899F6D8DEBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48482737-1790-BF4D-AC8C-AB13B943C873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19940" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
+    <workbookView xWindow="15560" yWindow="1480" windowWidth="18640" windowHeight="16900" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -496,7 +496,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -611,8 +611,12 @@
       <c r="F6" s="1">
         <v>5</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="G6" s="1">
+        <v>7821428</v>
+      </c>
+      <c r="H6" s="1">
+        <v>340921788</v>
+      </c>
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -634,8 +638,12 @@
       <c r="F7" s="1">
         <v>5</v>
       </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="G7" s="1">
+        <v>19647428</v>
+      </c>
+      <c r="H7" s="1">
+        <v>352747788</v>
+      </c>
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -649,7 +657,7 @@
         <v>12</v>
       </c>
       <c r="D8" s="1">
-        <v>126</v>
+        <v>80</v>
       </c>
       <c r="E8" s="1">
         <v>333100360</v>
@@ -657,8 +665,12 @@
       <c r="F8" s="1">
         <v>5</v>
       </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="G8" s="1">
+        <v>8541000</v>
+      </c>
+      <c r="H8" s="1">
+        <v>341641360</v>
+      </c>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -681,7 +693,9 @@
         <v>5</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="H9" s="1">
+        <v>334351788</v>
+      </c>
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -704,7 +718,9 @@
         <v>5</v>
       </c>
       <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="H10" s="1">
+        <v>332011617</v>
+      </c>
       <c r="I10" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
filled in all test cases
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxrice/PycharmProjects/cs151-lab2-max-and-jenna/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48482737-1790-BF4D-AC8C-AB13B943C873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A981E7-9B42-C14D-8297-C4C6B5FC4F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15560" yWindow="1480" windowWidth="18640" windowHeight="16900" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
+    <workbookView xWindow="7100" yWindow="3220" windowWidth="25220" windowHeight="17260" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Test Description</t>
   </si>
@@ -89,6 +89,15 @@
   </si>
   <si>
     <t>Population Low Birth Rate and Low Migration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">increase </t>
+  </si>
+  <si>
+    <t>increase</t>
+  </si>
+  <si>
+    <t>decrease</t>
   </si>
 </sst>
 </file>
@@ -496,7 +505,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -617,7 +626,9 @@
       <c r="H6" s="1">
         <v>340921788</v>
       </c>
-      <c r="I6" s="1"/>
+      <c r="I6" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -644,7 +655,9 @@
       <c r="H7" s="1">
         <v>352747788</v>
       </c>
-      <c r="I7" s="1"/>
+      <c r="I7" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -671,7 +684,9 @@
       <c r="H8" s="1">
         <v>341641360</v>
       </c>
-      <c r="I8" s="1"/>
+      <c r="I8" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -681,7 +696,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D9" s="1">
         <v>126</v>
@@ -692,11 +707,15 @@
       <c r="F9" s="1">
         <v>5</v>
       </c>
-      <c r="G9" s="1"/>
+      <c r="G9" s="1">
+        <v>57878572</v>
+      </c>
       <c r="H9" s="1">
-        <v>334351788</v>
-      </c>
-      <c r="I9" s="1"/>
+        <v>275221788</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
@@ -717,11 +736,15 @@
       <c r="F10" s="1">
         <v>5</v>
       </c>
-      <c r="G10" s="1"/>
+      <c r="G10" s="1">
+        <v>1088743</v>
+      </c>
       <c r="H10" s="1">
         <v>332011617</v>
       </c>
-      <c r="I10" s="1"/>
+      <c r="I10" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Worked with professor to push
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zee/development/CS151_labs/Lab2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxrice/PycharmProjects/cs151-lab2-max-and-jenna/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C084CA8B-2F93-D948-9FA4-65E66A2852B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48482737-1790-BF4D-AC8C-AB13B943C873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="67920" windowHeight="28300" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
+    <workbookView xWindow="15560" yWindow="1480" windowWidth="18640" windowHeight="16900" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -164,14 +164,14 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -197,9 +197,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -237,7 +237,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -343,7 +343,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -485,7 +485,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -496,7 +496,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:I10"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -509,44 +509,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <f>60*60*24*365</f>
         <v>31536000</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -564,98 +564,164 @@
       <c r="I4" s="5"/>
     </row>
     <row r="5" spans="1:9" ht="76" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="B6" s="1">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1">
+        <v>126</v>
+      </c>
+      <c r="E6" s="1">
+        <v>333100360</v>
+      </c>
+      <c r="F6" s="1">
+        <v>5</v>
+      </c>
+      <c r="G6" s="1">
+        <v>7821428</v>
+      </c>
+      <c r="H6" s="1">
+        <v>340921788</v>
+      </c>
+      <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
+      <c r="B7" s="1">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1">
+        <v>126</v>
+      </c>
+      <c r="E7" s="1">
+        <v>333100360</v>
+      </c>
+      <c r="F7" s="1">
+        <v>5</v>
+      </c>
+      <c r="G7" s="1">
+        <v>19647428</v>
+      </c>
+      <c r="H7" s="1">
+        <v>352747788</v>
+      </c>
+      <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
+      <c r="B8" s="1">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1">
+        <v>80</v>
+      </c>
+      <c r="E8" s="1">
+        <v>333100360</v>
+      </c>
+      <c r="F8" s="1">
+        <v>5</v>
+      </c>
+      <c r="G8" s="1">
+        <v>8541000</v>
+      </c>
+      <c r="H8" s="1">
+        <v>341641360</v>
+      </c>
+      <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+      <c r="B9" s="1">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1">
+        <v>126</v>
+      </c>
+      <c r="E9" s="1">
+        <v>333100360</v>
+      </c>
+      <c r="F9" s="1">
+        <v>5</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1">
+        <v>334351788</v>
+      </c>
+      <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="B10" s="1">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1">
+        <v>12</v>
+      </c>
+      <c r="D10" s="1">
+        <v>200</v>
+      </c>
+      <c r="E10" s="1">
+        <v>333100360</v>
+      </c>
+      <c r="F10" s="1">
+        <v>5</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1">
+        <v>332011617</v>
+      </c>
+      <c r="I10" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>